<commit_message>
minor updates to output formatting
</commit_message>
<xml_diff>
--- a/examples/WOMBAT_baselines.xlsx
+++ b/examples/WOMBAT_baselines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rhammond/Documents/GitHub/WOMBAT/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141E0B31-886A-3A41-907D-BD1D2761A303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BA619C-2D4D-3F45-BC3F-4E910B35170F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7660" yWindow="460" windowWidth="43540" windowHeight="24840" activeTab="2" xr2:uid="{FC377038-10D9-45F3-8213-AE0CAB167905}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="132">
   <si>
     <t>power_curve: 2016CACost_NREL_Reference_6MW_155.csv</t>
   </si>
@@ -352,18 +352,12 @@
     <t>Materials Cost</t>
   </si>
   <si>
-    <t>Millions USD$</t>
-  </si>
-  <si>
     <t>Total Servicing Equipment Cost</t>
   </si>
   <si>
     <t>Cable Repair Truck Cost</t>
   </si>
   <si>
-    <t>Milllions USD$</t>
-  </si>
-  <si>
     <t>Crawler Crane Cost</t>
   </si>
   <si>
@@ -403,12 +397,6 @@
     <t>Year 20</t>
   </si>
   <si>
-    <t>````````````````````````````</t>
-  </si>
-  <si>
-    <t></t>
-  </si>
-  <si>
     <t>Cable Laying Vessel Cost</t>
   </si>
   <si>
@@ -443,6 +431,9 @@
   </si>
   <si>
     <t>Jack-up Vessel Utilization</t>
+  </si>
+  <si>
+    <t>USD$/kW</t>
   </si>
 </sst>
 </file>
@@ -4371,18 +4362,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B462E31A-B89C-6C4B-96F6-9A1C6E45F83C}">
-  <dimension ref="A1:W35"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U40" sqref="U40"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="23" width="11.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="23" width="12.83203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
@@ -4432,28 +4422,28 @@
         <v>93</v>
       </c>
       <c r="P1" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="R1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="V1" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -4464,67 +4454,67 @@
         <v>96</v>
       </c>
       <c r="C2" s="8">
-        <v>44.277812434116854</v>
+        <v>38.933472825098121</v>
       </c>
       <c r="D2" s="8">
-        <v>89.114502051904509</v>
+        <v>90.883619443962786</v>
       </c>
       <c r="E2" s="8">
-        <v>78.392433963354719</v>
+        <v>72.235564418241722</v>
       </c>
       <c r="F2" s="8">
-        <v>75.076952341426292</v>
+        <v>61.289657835881115</v>
       </c>
       <c r="G2" s="8">
-        <v>70.014016530836358</v>
+        <v>49.636437200161843</v>
       </c>
       <c r="H2" s="8">
-        <v>60.248107045835496</v>
+        <v>39.449309288480435</v>
       </c>
       <c r="I2" s="8">
-        <v>55.283509623721173</v>
+        <v>32.969048031905665</v>
       </c>
       <c r="J2" s="8">
-        <v>48.360079315671761</v>
+        <v>32.804754328929469</v>
       </c>
       <c r="K2" s="8">
-        <v>44.96387492052483</v>
+        <v>33.167591468701232</v>
       </c>
       <c r="L2" s="8">
-        <v>38.887347552164613</v>
+        <v>33.770446794982952</v>
       </c>
       <c r="M2" s="8">
-        <v>32.579330674527483</v>
+        <v>34.766920987226172</v>
       </c>
       <c r="N2" s="8">
-        <v>28.278976735606744</v>
+        <v>33.300189066426874</v>
       </c>
       <c r="O2" s="8">
-        <v>28.291717241777931</v>
+        <v>31.513929830645626</v>
       </c>
       <c r="P2" s="8">
-        <v>30.944309577481071</v>
+        <v>31.205421651927633</v>
       </c>
       <c r="Q2" s="8">
-        <v>23.89688457314606</v>
+        <v>30.88202994046587</v>
       </c>
       <c r="R2" s="8">
-        <v>21.866858038781675</v>
+        <v>29.190588181042632</v>
       </c>
       <c r="S2" s="8">
-        <v>27.036442980174556</v>
+        <v>27.79131264088781</v>
       </c>
       <c r="T2" s="8">
-        <v>30.916999017397838</v>
+        <v>29.049043407895496</v>
       </c>
       <c r="U2" s="8">
-        <v>34.804780070516159</v>
+        <v>28.493006184613606</v>
       </c>
       <c r="V2" s="8">
-        <v>34.399858200179843</v>
+        <v>27.235941066611328</v>
       </c>
       <c r="W2" s="8">
-        <v>32.235997919195427</v>
+        <v>29.064360441592974</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
@@ -4535,67 +4525,67 @@
         <v>96</v>
       </c>
       <c r="C3" s="8">
-        <v>43.862928747479515</v>
+        <v>38.806451591064935</v>
       </c>
       <c r="D3" s="8">
-        <v>89.43907335818345</v>
+        <v>91.148248984037082</v>
       </c>
       <c r="E3" s="8">
-        <v>78.440516383696661</v>
+        <v>72.820987995169332</v>
       </c>
       <c r="F3" s="8">
-        <v>75.139277694375011</v>
+        <v>61.412284458710019</v>
       </c>
       <c r="G3" s="8">
-        <v>69.696637703994668</v>
+        <v>49.551942027162887</v>
       </c>
       <c r="H3" s="8">
-        <v>60.463759943321918</v>
+        <v>39.564668737433287</v>
       </c>
       <c r="I3" s="8">
-        <v>54.992548052813916</v>
+        <v>32.842817630149568</v>
       </c>
       <c r="J3" s="8">
-        <v>47.843553125271363</v>
+        <v>32.577847688939052</v>
       </c>
       <c r="K3" s="8">
-        <v>45.079834085817552</v>
+        <v>33.036846468421111</v>
       </c>
       <c r="L3" s="8">
-        <v>38.796560661567561</v>
+        <v>33.747746101840647</v>
       </c>
       <c r="M3" s="8">
-        <v>32.622065472352993</v>
+        <v>34.817436351719948</v>
       </c>
       <c r="N3" s="8">
-        <v>28.042231119082615</v>
+        <v>32.997204910065939</v>
       </c>
       <c r="O3" s="8">
-        <v>27.959882468239666</v>
+        <v>31.287578514428471</v>
       </c>
       <c r="P3" s="8">
-        <v>30.720245241061122</v>
+        <v>31.024493921418699</v>
       </c>
       <c r="Q3" s="8">
-        <v>23.671664202650391</v>
+        <v>30.600656371058292</v>
       </c>
       <c r="R3" s="8">
-        <v>21.693251410291126</v>
+        <v>29.251220135403948</v>
       </c>
       <c r="S3" s="8">
-        <v>26.779722646410381</v>
+        <v>27.671663289765299</v>
       </c>
       <c r="T3" s="8">
-        <v>30.683724274408679</v>
+        <v>28.893872819699169</v>
       </c>
       <c r="U3" s="8">
-        <v>34.734925743522957</v>
+        <v>28.384853454517579</v>
       </c>
       <c r="V3" s="8">
-        <v>34.454213101884321</v>
+        <v>27.178419652688063</v>
       </c>
       <c r="W3" s="8">
-        <v>32.069471007295306</v>
+        <v>28.825718815907521</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
@@ -4606,67 +4596,67 @@
         <v>99</v>
       </c>
       <c r="C4" s="8">
-        <v>7793755.9234999986</v>
+        <v>6895299.0736000007</v>
       </c>
       <c r="D4" s="8">
-        <v>768948.59</v>
+        <v>783643.15400000021</v>
       </c>
       <c r="E4" s="8">
-        <v>718328.06669999973</v>
+        <v>666866.58799999999</v>
       </c>
       <c r="F4" s="8">
-        <v>703222.59699999995</v>
+        <v>574752.74569999985</v>
       </c>
       <c r="G4" s="8">
-        <v>584303.78200000001</v>
+        <v>415420.14199999999</v>
       </c>
       <c r="H4" s="8">
-        <v>516742.42200000002</v>
+        <v>338132.1765</v>
       </c>
       <c r="I4" s="8">
-        <v>461054.38500000001</v>
+        <v>275352.30900000001</v>
       </c>
       <c r="J4" s="8">
-        <v>412613.69900000002</v>
+        <v>280958.77839999989</v>
       </c>
       <c r="K4" s="8">
-        <v>361333.08199999999</v>
+        <v>264803.67099999997</v>
       </c>
       <c r="L4" s="8">
-        <v>350039.45299999998</v>
+        <v>304486.85100000002</v>
       </c>
       <c r="M4" s="8">
-        <v>257923.272</v>
+        <v>275280.76400000002</v>
       </c>
       <c r="N4" s="8">
-        <v>259673.74100000001</v>
+        <v>305557.272</v>
       </c>
       <c r="O4" s="8">
-        <v>249227.22899999999</v>
+        <v>278889.45899999997</v>
       </c>
       <c r="P4" s="8">
-        <v>277752.10499999998</v>
+        <v>280502.92</v>
       </c>
       <c r="Q4" s="8">
-        <v>229331.342</v>
+        <v>296459.49400000001</v>
       </c>
       <c r="R4" s="8">
-        <v>203494.03099999999</v>
+        <v>274391.72600000002</v>
       </c>
       <c r="S4" s="8">
-        <v>241534.19500000001</v>
+        <v>249578.87</v>
       </c>
       <c r="T4" s="8">
-        <v>286864.65399999998</v>
+        <v>270131.18599999999</v>
       </c>
       <c r="U4" s="8">
-        <v>298396.28939999989</v>
+        <v>243844.913</v>
       </c>
       <c r="V4" s="8">
-        <v>315620.06139999995</v>
+        <v>248969.682</v>
       </c>
       <c r="W4" s="8">
-        <v>297352.92700000003</v>
+        <v>267276.37199999997</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
@@ -4677,67 +4667,67 @@
         <v>96</v>
       </c>
       <c r="C5" s="8">
-        <v>21.642872433736965</v>
+        <v>19.147902462843849</v>
       </c>
       <c r="D5" s="8">
-        <v>42.735890655497904</v>
+        <v>43.552571105271817</v>
       </c>
       <c r="E5" s="8">
-        <v>39.922551536594149</v>
+        <v>37.062474601290276</v>
       </c>
       <c r="F5" s="8">
-        <v>38.976249915753698</v>
+        <v>31.855783292141332</v>
       </c>
       <c r="G5" s="8">
-        <v>32.473877788300364</v>
+        <v>23.087824069751413</v>
       </c>
       <c r="H5" s="8">
-        <v>28.719017019914368</v>
+        <v>18.792387306425152</v>
       </c>
       <c r="I5" s="8">
-        <v>25.624040462312092</v>
+        <v>15.303267763535233</v>
       </c>
       <c r="J5" s="8">
-        <v>22.869194931299361</v>
+        <v>15.572195219066973</v>
       </c>
       <c r="K5" s="8">
-        <v>20.081825083476723</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>121</v>
+        <v>14.717005631066232</v>
+      </c>
+      <c r="L5" s="8">
+        <v>16.922479525416495</v>
       </c>
       <c r="M5" s="8">
-        <v>14.334613383841752</v>
+        <v>15.299291503825927</v>
       </c>
       <c r="N5" s="8">
-        <v>14.392467860037636</v>
+        <v>16.935571535747922</v>
       </c>
       <c r="O5" s="8">
-        <v>13.851313007696309</v>
+        <v>15.499852109482331</v>
       </c>
       <c r="P5" s="8">
-        <v>15.436641334649398</v>
+        <v>15.589523504644017</v>
       </c>
       <c r="Q5" s="8">
-        <v>12.745558393690004</v>
+        <v>16.476342741415571</v>
       </c>
       <c r="R5" s="8">
-        <v>11.278696450393118</v>
+        <v>15.208215055966146</v>
       </c>
       <c r="S5" s="8">
-        <v>13.423756908226736</v>
+        <v>13.870856175498972</v>
       </c>
       <c r="T5" s="8">
-        <v>15.943089883643896</v>
+        <v>15.013093173804981</v>
       </c>
       <c r="U5" s="8">
-        <v>16.583984107188108</v>
+        <v>13.552179787295533</v>
       </c>
       <c r="V5" s="8">
-        <v>17.493303605475475</v>
+        <v>13.799193297364598</v>
       </c>
       <c r="W5" s="8">
-        <v>16.525997107770564</v>
+        <v>14.85443104667138</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
@@ -4819,67 +4809,67 @@
         <v>96</v>
       </c>
       <c r="C7" s="8">
-        <v>97.901295294310543</v>
+        <v>98.193332091637174</v>
       </c>
       <c r="D7" s="8">
-        <v>85.834738617200685</v>
+        <v>83.495145631067956</v>
       </c>
       <c r="E7" s="8">
-        <v>85.689948892674622</v>
+        <v>98.467432950191565</v>
       </c>
       <c r="F7" s="8">
-        <v>98.35164835164835</v>
+        <v>92.825112107623326</v>
       </c>
       <c r="G7" s="8">
-        <v>96.320346320346317</v>
+        <v>94.848484848484844</v>
       </c>
       <c r="H7" s="8">
-        <v>93.540669856459331</v>
+        <v>102.36486486486487</v>
       </c>
       <c r="I7" s="8">
-        <v>96.938775510204081</v>
+        <v>110.48034934497817</v>
       </c>
       <c r="J7" s="8">
-        <v>101.49253731343283</v>
+        <v>110.85972850678733</v>
       </c>
       <c r="K7" s="8">
-        <v>101.33333333333334</v>
+        <v>105.26315789473684</v>
       </c>
       <c r="L7" s="8">
-        <v>105.44747081712063</v>
+        <v>100</v>
       </c>
       <c r="M7" s="8">
-        <v>109.21052631578947</v>
+        <v>99.606299212598429</v>
       </c>
       <c r="N7" s="8">
-        <v>111.42857142857143</v>
+        <v>99.583333333333329</v>
       </c>
       <c r="O7" s="8">
-        <v>122.43589743589745</v>
+        <v>99.180327868852459</v>
       </c>
       <c r="P7" s="8">
-        <v>98.113207547169807</v>
+        <v>101.47058823529412</v>
       </c>
       <c r="Q7" s="8">
-        <v>97.484276729559753</v>
+        <v>98.666666666666671</v>
       </c>
       <c r="R7" s="8">
-        <v>101.47058823529412</v>
+        <v>99.465240641711233</v>
       </c>
       <c r="S7" s="8">
+        <v>100.51282051282051</v>
+      </c>
+      <c r="T7" s="8">
         <v>100</v>
       </c>
-      <c r="T7" s="8">
-        <v>101.00502512562815</v>
-      </c>
       <c r="U7" s="8">
-        <v>103.78151260504202</v>
+        <v>98.039215686274503</v>
       </c>
       <c r="V7" s="8">
-        <v>98.4375</v>
+        <v>100</v>
       </c>
       <c r="W7" s="8">
-        <v>100.44843049327355</v>
+        <v>102.24719101123596</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
@@ -4887,359 +4877,359 @@
         <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="C8" s="8">
-        <v>35.109146000000003</v>
+        <v>167.60504868549171</v>
       </c>
       <c r="D8" s="8">
-        <v>1.447184</v>
+        <v>7.3386660175267773</v>
       </c>
       <c r="E8" s="8">
-        <v>1.5112989999999999</v>
+        <v>7.8033495618305748</v>
       </c>
       <c r="F8" s="8">
-        <v>1.6441669999999999</v>
+        <v>8.8127702044790652</v>
       </c>
       <c r="G8" s="8">
-        <v>2.031955</v>
+        <v>8.1477117818889973</v>
       </c>
       <c r="H8" s="8">
-        <v>1.795479</v>
+        <v>10.602755598831548</v>
       </c>
       <c r="I8" s="8">
-        <v>1.872808</v>
+        <v>10.802458617332036</v>
       </c>
       <c r="J8" s="8">
-        <v>2.0960359999999998</v>
+        <v>10.967341772151899</v>
       </c>
       <c r="K8" s="8">
-        <v>2.2643580000000001</v>
+        <v>8.3335783836416741</v>
       </c>
       <c r="L8" s="8">
-        <v>2.0831110000000002</v>
+        <v>9.1706962025316461</v>
       </c>
       <c r="M8" s="8">
-        <v>2.2806440000000001</v>
+        <v>9.0651168451801372</v>
       </c>
       <c r="N8" s="8">
-        <v>2.0992730000000002</v>
+        <v>7.6975219084712752</v>
       </c>
       <c r="O8" s="8">
-        <v>2.0163250000000001</v>
+        <v>7.6813339824732232</v>
       </c>
       <c r="P8" s="8">
-        <v>1.7106410000000001</v>
+        <v>7.7167624148003897</v>
       </c>
       <c r="Q8" s="8">
-        <v>1.389926</v>
+        <v>7.6116260954235635</v>
       </c>
       <c r="R8" s="8">
-        <v>1.402989</v>
+        <v>7.4646981499513148</v>
       </c>
       <c r="S8" s="8">
-        <v>1.4731559999999999</v>
+        <v>7.7642405063291138</v>
       </c>
       <c r="T8" s="8">
-        <v>1.4212610000000001</v>
+        <v>7.6125121713729307</v>
       </c>
       <c r="U8" s="8">
-        <v>1.6988030000000001</v>
+        <v>9.2518062317429415</v>
       </c>
       <c r="V8" s="8">
-        <v>1.366241</v>
+        <v>7.1171908471275556</v>
       </c>
       <c r="W8" s="8">
-        <v>1.50349</v>
+        <v>6.6429113924050629</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="C9" s="8">
-        <v>50.347529166659008</v>
+        <v>246.2797590068111</v>
       </c>
       <c r="D9" s="8">
-        <v>2.3954624999880032</v>
+        <v>12.331852482882189</v>
       </c>
       <c r="E9" s="8">
-        <v>2.3821000000040007</v>
+        <v>12.757708536207401</v>
       </c>
       <c r="F9" s="8">
-        <v>2.694699999988003</v>
+        <v>12.445796819196694</v>
       </c>
       <c r="G9" s="8">
-        <v>2.4529333333279988</v>
+        <v>11.650113599479061</v>
       </c>
       <c r="H9" s="8">
-        <v>2.4362666666679997</v>
+        <v>12.433138591397276</v>
       </c>
       <c r="I9" s="8">
-        <v>2.5196000000109984</v>
+        <v>12.266796494678669</v>
       </c>
       <c r="J9" s="8">
-        <v>2.7422000000000004</v>
+        <v>12.652710158987347</v>
       </c>
       <c r="K9" s="8">
-        <v>2.6754333333329989</v>
+        <v>11.767770204444984</v>
       </c>
       <c r="L9" s="8">
-        <v>2.3962666666700008</v>
+        <v>12.863193768247326</v>
       </c>
       <c r="M9" s="8">
-        <v>2.5812666666630002</v>
+        <v>13.341934436898727</v>
       </c>
       <c r="N9" s="8">
-        <v>2.5730333333379996</v>
+        <v>11.946770529050637</v>
       </c>
       <c r="O9" s="8">
-        <v>2.5137666666710001</v>
+        <v>11.666342096762412</v>
       </c>
       <c r="P9" s="8">
-        <v>2.716266666666999</v>
+        <v>11.954397922789672</v>
       </c>
       <c r="Q9" s="8">
-        <v>2.4221000000029989</v>
+        <v>12.542680947755599</v>
       </c>
       <c r="R9" s="8">
-        <v>2.4372000000029996</v>
+        <v>11.865628042833498</v>
       </c>
       <c r="S9" s="8">
-        <v>2.4395999999989999</v>
+        <v>12.449367088588126</v>
       </c>
       <c r="T9" s="8">
-        <v>2.4729333333320018</v>
+        <v>12.753651411874392</v>
       </c>
       <c r="U9" s="8">
-        <v>2.6979333333279998</v>
+        <v>12.351996105160664</v>
       </c>
       <c r="V9" s="8">
-        <v>2.3622000000009984</v>
+        <v>12.279454722502436</v>
       </c>
       <c r="W9" s="8">
-        <v>2.4362666666640003</v>
+        <v>11.958455047074004</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="C10" s="8">
-        <v>3.512</v>
+        <v>17.098344693281401</v>
       </c>
       <c r="D10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="E10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="F10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="G10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="H10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="I10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="J10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="K10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="L10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="M10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="N10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="O10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="P10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="Q10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="R10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="S10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="T10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="U10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="V10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
       <c r="W10" s="8">
-        <v>0.17560000000000001</v>
+        <v>0.8549172346640701</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="C11" s="8">
-        <v>46.104999999983015</v>
+        <v>225.624797143705</v>
       </c>
       <c r="D11" s="8">
-        <v>2.1833333333330001</v>
+        <v>11.299091204152873</v>
       </c>
       <c r="E11" s="8">
-        <v>2.1699999999970001</v>
+        <v>11.725089256718599</v>
       </c>
       <c r="F11" s="8">
-        <v>2.4824999999999999</v>
+        <v>11.412690684844206</v>
       </c>
       <c r="G11" s="8">
-        <v>2.2408333333330002</v>
+        <v>10.617494320024344</v>
       </c>
       <c r="H11" s="8">
-        <v>2.2241666666679998</v>
+        <v>11.400519311908472</v>
       </c>
       <c r="I11" s="8">
-        <v>2.3075000000010002</v>
+        <v>11.234177215194743</v>
       </c>
       <c r="J11" s="8">
-        <v>2.5299999999999998</v>
+        <v>11.619604024664071</v>
       </c>
       <c r="K11" s="8">
-        <v>2.4633333333329999</v>
+        <v>10.735150925019473</v>
       </c>
       <c r="L11" s="8">
-        <v>2.1841666666680002</v>
+        <v>11.830574488807207</v>
       </c>
       <c r="M11" s="8">
-        <v>2.3691666666630002</v>
+        <v>12.309315157395329</v>
       </c>
       <c r="N11" s="8">
-        <v>2.3608333333330003</v>
+        <v>10.913664394683543</v>
       </c>
       <c r="O11" s="8">
-        <v>2.3016666666679999</v>
+        <v>10.633722817268744</v>
       </c>
       <c r="P11" s="8">
-        <v>2.5041666666639997</v>
+        <v>10.921778643291136</v>
       </c>
       <c r="Q11" s="8">
-        <v>2.2099999999979993</v>
+        <v>11.5100616682814</v>
       </c>
       <c r="R11" s="8">
-        <v>2.2249999999979999</v>
+        <v>10.832521908461539</v>
       </c>
       <c r="S11" s="8">
-        <v>2.2274999999990004</v>
+        <v>11.416747809148005</v>
       </c>
       <c r="T11" s="8">
-        <v>2.2608333333310004</v>
+        <v>11.721032132414802</v>
       </c>
       <c r="U11" s="8">
-        <v>2.4858333333310005</v>
+        <v>11.319376825696205</v>
       </c>
       <c r="V11" s="8">
-        <v>2.15</v>
+        <v>11.246348588125608</v>
       </c>
       <c r="W11" s="8">
-        <v>2.224166666665</v>
+        <v>10.925835767604672</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="C12" s="8">
-        <v>0.73052916667599999</v>
+        <v>3.5566171698247326</v>
       </c>
       <c r="D12" s="8">
-        <v>3.6529166654999987E-2</v>
+        <v>0.17784404406523838</v>
       </c>
       <c r="E12" s="8">
-        <v>3.6500000007000002E-2</v>
+        <v>0.17770204482473206</v>
       </c>
       <c r="F12" s="8">
-        <v>3.6599999987999968E-2</v>
+        <v>0.17818889968841295</v>
       </c>
       <c r="G12" s="8">
-        <v>3.6499999995000004E-2</v>
+        <v>0.17770204479065249</v>
       </c>
       <c r="H12" s="8">
-        <v>3.6499999999999984E-2</v>
+        <v>0.17770204482473234</v>
       </c>
       <c r="I12" s="8">
-        <v>3.6500000010000019E-2</v>
+        <v>0.17770204481986376</v>
       </c>
       <c r="J12" s="8">
-        <v>3.6600000000000042E-2</v>
+        <v>0.17818889965920148</v>
       </c>
       <c r="K12" s="8">
-        <v>3.649999999999997E-2</v>
+        <v>0.177702044761441</v>
       </c>
       <c r="L12" s="8">
-        <v>3.6500000001999988E-2</v>
+        <v>0.17770204477604667</v>
       </c>
       <c r="M12" s="8">
-        <v>3.6500000000000046E-2</v>
+        <v>0.17770204483933796</v>
       </c>
       <c r="N12" s="8">
-        <v>3.6600000005000029E-2</v>
+        <v>0.17818889970301846</v>
       </c>
       <c r="O12" s="8">
-        <v>3.6500000002999994E-2</v>
+        <v>0.17770204482960072</v>
       </c>
       <c r="P12" s="8">
-        <v>3.6500000003000015E-2</v>
+        <v>0.17770204483446939</v>
       </c>
       <c r="Q12" s="8">
-        <v>3.6500000004999991E-2</v>
+        <v>0.17770204481012644</v>
       </c>
       <c r="R12" s="8">
-        <v>3.6600000004999994E-2</v>
+        <v>0.17818889970788704</v>
       </c>
       <c r="S12" s="8">
-        <v>3.649999999999997E-2</v>
+        <v>0.17770204477604681</v>
       </c>
       <c r="T12" s="8">
-        <v>3.6500000000999976E-2</v>
+        <v>0.17770204479552082</v>
       </c>
       <c r="U12" s="8">
-        <v>3.6499999997000016E-2</v>
+        <v>0.17770204480038942</v>
       </c>
       <c r="V12" s="8">
-        <v>3.6600000001000041E-2</v>
+        <v>0.17818889971275564</v>
       </c>
       <c r="W12" s="8">
-        <v>3.6499999998999985E-2</v>
+        <v>0.17770204480525809</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
         <v>96</v>
@@ -5257,49 +5247,49 @@
         <v>0</v>
       </c>
       <c r="G13" s="8">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0</v>
+      </c>
+      <c r="L13" s="8">
+        <v>0</v>
+      </c>
+      <c r="M13" s="8">
+        <v>0</v>
+      </c>
+      <c r="N13" s="8">
+        <v>0</v>
+      </c>
+      <c r="O13" s="8">
+        <v>0</v>
+      </c>
+      <c r="P13" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>0</v>
+      </c>
+      <c r="R13" s="8">
+        <v>0</v>
+      </c>
+      <c r="S13" s="8">
+        <v>0</v>
+      </c>
+      <c r="T13" s="8">
+        <v>0</v>
+      </c>
+      <c r="U13" s="8">
         <v>3.225806451612903</v>
-      </c>
-      <c r="H13" s="8">
-        <v>0</v>
-      </c>
-      <c r="I13" s="8">
-        <v>0</v>
-      </c>
-      <c r="J13" s="8">
-        <v>0</v>
-      </c>
-      <c r="K13" s="8">
-        <v>0</v>
-      </c>
-      <c r="L13" s="8">
-        <v>0</v>
-      </c>
-      <c r="M13" s="8">
-        <v>0</v>
-      </c>
-      <c r="N13" s="8">
-        <v>0</v>
-      </c>
-      <c r="O13" s="8">
-        <v>0</v>
-      </c>
-      <c r="P13" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="8">
-        <v>0</v>
-      </c>
-      <c r="R13" s="8">
-        <v>0</v>
-      </c>
-      <c r="S13" s="8">
-        <v>0</v>
-      </c>
-      <c r="T13" s="8">
-        <v>0</v>
-      </c>
-      <c r="U13" s="8">
-        <v>0</v>
       </c>
       <c r="V13" s="8">
         <v>0</v>
@@ -5310,13 +5300,13 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s">
         <v>96</v>
       </c>
       <c r="C14" s="8">
-        <v>4.8514851485148514</v>
+        <v>5.0196850393700787</v>
       </c>
       <c r="D14" s="8">
         <v>0</v>
@@ -5328,49 +5318,49 @@
         <v>0</v>
       </c>
       <c r="G14" s="8">
+        <v>0</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0</v>
+      </c>
+      <c r="K14" s="8">
+        <v>0</v>
+      </c>
+      <c r="L14" s="8">
+        <v>0</v>
+      </c>
+      <c r="M14" s="8">
+        <v>0</v>
+      </c>
+      <c r="N14" s="8">
+        <v>0</v>
+      </c>
+      <c r="O14" s="8">
+        <v>0</v>
+      </c>
+      <c r="P14" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>0</v>
+      </c>
+      <c r="R14" s="8">
+        <v>0</v>
+      </c>
+      <c r="S14" s="8">
+        <v>0</v>
+      </c>
+      <c r="T14" s="8">
+        <v>0</v>
+      </c>
+      <c r="U14" s="8">
         <v>100</v>
-      </c>
-      <c r="H14" s="8">
-        <v>0</v>
-      </c>
-      <c r="I14" s="8">
-        <v>0</v>
-      </c>
-      <c r="J14" s="8">
-        <v>0</v>
-      </c>
-      <c r="K14" s="8">
-        <v>0</v>
-      </c>
-      <c r="L14" s="8">
-        <v>0</v>
-      </c>
-      <c r="M14" s="8">
-        <v>0</v>
-      </c>
-      <c r="N14" s="8">
-        <v>0</v>
-      </c>
-      <c r="O14" s="8">
-        <v>0</v>
-      </c>
-      <c r="P14" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="8">
-        <v>0</v>
-      </c>
-      <c r="R14" s="8">
-        <v>0</v>
-      </c>
-      <c r="S14" s="8">
-        <v>0</v>
-      </c>
-      <c r="T14" s="8">
-        <v>0</v>
-      </c>
-      <c r="U14" s="8">
-        <v>0</v>
       </c>
       <c r="V14" s="8">
         <v>0</v>
@@ -5381,13 +5371,13 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B15" t="s">
         <v>96</v>
       </c>
       <c r="C15" s="8">
-        <v>4.9555099247091032</v>
+        <v>3.0390143737166326</v>
       </c>
       <c r="D15" s="8">
         <v>0</v>
@@ -5399,7 +5389,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="8">
-        <v>99.178082191780831</v>
+        <v>0</v>
       </c>
       <c r="H15" s="8">
         <v>0</v>
@@ -5441,18 +5431,13 @@
         <v>0</v>
       </c>
       <c r="U15" s="8">
-        <v>0</v>
+        <v>60.821917808219183</v>
       </c>
       <c r="V15" s="8">
         <v>0</v>
       </c>
       <c r="W15" s="8">
         <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E35" s="8" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -5466,16 +5451,14 @@
   <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="23" width="11" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="23" width="12.83203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
@@ -5525,28 +5508,28 @@
         <v>93</v>
       </c>
       <c r="P1" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="R1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="V1" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -5557,67 +5540,67 @@
         <v>96</v>
       </c>
       <c r="C2" s="8">
-        <v>31.612476621022157</v>
+        <v>30.194556130722809</v>
       </c>
       <c r="D2" s="8">
-        <v>89.885229540918161</v>
+        <v>87.843491099991795</v>
       </c>
       <c r="E2" s="8">
-        <v>72.538689743800063</v>
+        <v>67.081521887731384</v>
       </c>
       <c r="F2" s="8">
-        <v>57.874551443560961</v>
+        <v>55.366043868547052</v>
       </c>
       <c r="G2" s="8">
-        <v>48.933297787985673</v>
+        <v>44.150602903781476</v>
       </c>
       <c r="H2" s="8">
-        <v>41.553400049216634</v>
+        <v>36.652995379104802</v>
       </c>
       <c r="I2" s="8">
-        <v>37.059852896945834</v>
+        <v>33.027574987012272</v>
       </c>
       <c r="J2" s="8">
-        <v>31.283948496449725</v>
+        <v>31.593370635777624</v>
       </c>
       <c r="K2" s="8">
-        <v>27.135591830038553</v>
+        <v>29.689319990156669</v>
       </c>
       <c r="L2" s="8">
-        <v>23.725220791294124</v>
+        <v>25.451357558854891</v>
       </c>
       <c r="M2" s="8">
-        <v>20.354701555792523</v>
+        <v>22.682033193886202</v>
       </c>
       <c r="N2" s="8">
-        <v>18.959894418812649</v>
+        <v>22.456725892477341</v>
       </c>
       <c r="O2" s="8">
-        <v>19.288272769529435</v>
+        <v>21.936196100948788</v>
       </c>
       <c r="P2" s="8">
-        <v>19.756446012085419</v>
+        <v>19.386090832034562</v>
       </c>
       <c r="Q2" s="8">
-        <v>21.447379214174394</v>
+        <v>17.602603013151779</v>
       </c>
       <c r="R2" s="8">
-        <v>21.092378085359336</v>
+        <v>15.099786765267279</v>
       </c>
       <c r="S2" s="8">
-        <v>20.019823366964701</v>
+        <v>14.854947638968637</v>
       </c>
       <c r="T2" s="8">
-        <v>18.076449840045935</v>
+        <v>14.690687118912859</v>
       </c>
       <c r="U2" s="8">
-        <v>15.715418478112269</v>
+        <v>14.981543761791485</v>
       </c>
       <c r="V2" s="8">
-        <v>14.000346301931657</v>
+        <v>14.29483928318227</v>
       </c>
       <c r="W2" s="8">
-        <v>13.589328192929209</v>
+        <v>15.082711289749268</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
@@ -5628,67 +5611,67 @@
         <v>96</v>
       </c>
       <c r="C3" s="8">
-        <v>31.561509302933029</v>
+        <v>30.207346621591569</v>
       </c>
       <c r="D3" s="8">
-        <v>90.224045683526725</v>
+        <v>88.169824805877411</v>
       </c>
       <c r="E3" s="8">
-        <v>72.810461301663906</v>
+        <v>67.455463982696244</v>
       </c>
       <c r="F3" s="8">
-        <v>58.053115897717198</v>
+        <v>55.63675210980572</v>
       </c>
       <c r="G3" s="8">
-        <v>48.874392064773005</v>
+        <v>44.184565347302126</v>
       </c>
       <c r="H3" s="8">
-        <v>41.639498520862269</v>
+        <v>36.835126695905736</v>
       </c>
       <c r="I3" s="8">
-        <v>37.187440869242252</v>
+        <v>33.09423576694347</v>
       </c>
       <c r="J3" s="8">
-        <v>31.345990864573686</v>
+        <v>31.597621467663988</v>
       </c>
       <c r="K3" s="8">
-        <v>27.122757923269504</v>
+        <v>29.589559384867627</v>
       </c>
       <c r="L3" s="8">
-        <v>23.712488135779218</v>
+        <v>25.488842007974693</v>
       </c>
       <c r="M3" s="8">
-        <v>20.09492554763068</v>
+        <v>22.779754211018979</v>
       </c>
       <c r="N3" s="8">
-        <v>18.855886321176897</v>
+        <v>22.336725934700809</v>
       </c>
       <c r="O3" s="8">
-        <v>19.226656274495063</v>
+        <v>21.835301321910919</v>
       </c>
       <c r="P3" s="8">
-        <v>19.783280703673356</v>
+        <v>19.439986282996195</v>
       </c>
       <c r="Q3" s="8">
-        <v>21.371533249736764</v>
+        <v>17.664768285466316</v>
       </c>
       <c r="R3" s="8">
-        <v>21.07413605023946</v>
+        <v>15.142495018499226</v>
       </c>
       <c r="S3" s="8">
-        <v>19.957515195291723</v>
+        <v>14.741333867972067</v>
       </c>
       <c r="T3" s="8">
-        <v>17.99581376216873</v>
+        <v>14.691412943365354</v>
       </c>
       <c r="U3" s="8">
-        <v>15.830869955952926</v>
+        <v>15.048984218056615</v>
       </c>
       <c r="V3" s="8">
-        <v>13.948715471424222</v>
+        <v>14.294740973737319</v>
       </c>
       <c r="W3" s="8">
-        <v>13.551699103044543</v>
+        <v>15.133193994464195</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
@@ -5699,67 +5682,67 @@
         <v>99</v>
       </c>
       <c r="C4" s="8">
-        <v>29321224.238599997</v>
+        <v>28063182.132499997</v>
       </c>
       <c r="D4" s="8">
-        <v>3995338.4580000001</v>
+        <v>3904372.6005999981</v>
       </c>
       <c r="E4" s="8">
-        <v>3407374.4240000001</v>
+        <v>3156771.961399992</v>
       </c>
       <c r="F4" s="8">
-        <v>2740495.732499999</v>
+        <v>2626427.1842999952</v>
       </c>
       <c r="G4" s="8">
-        <v>2204893.5106000016</v>
+        <v>1993319.145</v>
       </c>
       <c r="H4" s="8">
-        <v>2022783.325</v>
+        <v>1789394.2699000014</v>
       </c>
       <c r="I4" s="8">
-        <v>1789939.074</v>
+        <v>1592921.2749999999</v>
       </c>
       <c r="J4" s="8">
-        <v>1485203.3835000005</v>
+        <v>1497125.885</v>
       </c>
       <c r="K4" s="8">
-        <v>1250582.0179999999</v>
+        <v>1364321.8359999999</v>
       </c>
       <c r="L4" s="8">
-        <v>1143477.9339999999</v>
+        <v>1229138.344</v>
       </c>
       <c r="M4" s="8">
-        <v>965937.86399999878</v>
+        <v>1094994.21</v>
       </c>
       <c r="N4" s="8">
-        <v>829534.66599999997</v>
+        <v>982668.65700000001</v>
       </c>
       <c r="O4" s="8">
-        <v>896405.228</v>
+        <v>1018028.199</v>
       </c>
       <c r="P4" s="8">
-        <v>960957.48600000003</v>
+        <v>944282.22629999998</v>
       </c>
       <c r="Q4" s="8">
-        <v>930260.397</v>
+        <v>768912.28</v>
       </c>
       <c r="R4" s="8">
-        <v>897715.43400000001</v>
+        <v>645039.56200000003</v>
       </c>
       <c r="S4" s="8">
-        <v>960718.37600000005</v>
+        <v>709620.92200000002</v>
       </c>
       <c r="T4" s="8">
-        <v>821531.00699999998</v>
+        <v>670681.05000000005</v>
       </c>
       <c r="U4" s="8">
-        <v>711154.52</v>
+        <v>676030.64</v>
       </c>
       <c r="V4" s="8">
-        <v>656282.71400000004</v>
+        <v>672563.10600000003</v>
       </c>
       <c r="W4" s="8">
-        <v>650638.68700000003</v>
+        <v>726568.77899999998</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
@@ -5770,67 +5753,67 @@
         <v>96</v>
       </c>
       <c r="C5" s="8">
-        <v>16.691021469836965</v>
+        <v>15.974884666270928</v>
       </c>
       <c r="D5" s="8">
-        <v>45.517850805238844</v>
+        <v>44.481500476216517</v>
       </c>
       <c r="E5" s="8">
-        <v>38.819329651199887</v>
+        <v>35.964281042936953</v>
       </c>
       <c r="F5" s="8">
-        <v>31.136449011130747</v>
+        <v>29.840446432953765</v>
       </c>
       <c r="G5" s="8">
-        <v>25.119777688914414</v>
+        <v>22.709366028217538</v>
       </c>
       <c r="H5" s="8">
-        <v>23.045043759512936</v>
+        <v>20.386103021126697</v>
       </c>
       <c r="I5" s="8">
-        <v>20.392309832390016</v>
+        <v>18.147737344944812</v>
       </c>
       <c r="J5" s="8">
-        <v>16.874304481883229</v>
+        <v>17.009763317172578</v>
       </c>
       <c r="K5" s="8">
-        <v>14.247555323143665</v>
+        <v>15.543363455736928</v>
       </c>
       <c r="L5" s="8">
-        <v>13.027346380298763</v>
+        <v>14.003253128446305</v>
       </c>
       <c r="M5" s="8">
-        <v>11.004678588029419</v>
+        <v>12.474983936237114</v>
       </c>
       <c r="N5" s="8">
-        <v>9.4248509583746891</v>
+        <v>11.164699937556581</v>
       </c>
       <c r="O5" s="8">
-        <v>10.212511369954155</v>
+        <v>11.598130212178383</v>
       </c>
       <c r="P5" s="8">
-        <v>10.947938438192109</v>
+        <v>10.757961546085911</v>
       </c>
       <c r="Q5" s="8">
-        <v>10.598214495666202</v>
+        <v>8.7600174081061617</v>
       </c>
       <c r="R5" s="8">
-        <v>10.199494385545849</v>
+        <v>7.3286891835636565</v>
       </c>
       <c r="S5" s="8">
-        <v>10.945214320218012</v>
+        <v>8.0845264038133777</v>
       </c>
       <c r="T5" s="8">
-        <v>9.3594888647362797</v>
+        <v>7.6408945807016115</v>
       </c>
       <c r="U5" s="8">
-        <v>8.1019982865319591</v>
+        <v>7.701841066724997</v>
       </c>
       <c r="V5" s="8">
-        <v>7.4564295134685104</v>
+        <v>7.641401009456497</v>
       </c>
       <c r="W5" s="8">
-        <v>7.4125571573747484</v>
+        <v>8.2776089259836478</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
@@ -5912,67 +5895,67 @@
         <v>96</v>
       </c>
       <c r="C7" s="8">
-        <v>96.415886341620933</v>
+        <v>96.457489878542518</v>
       </c>
       <c r="D7" s="8">
-        <v>62.939796716184517</v>
+        <v>60.866078588612673</v>
       </c>
       <c r="E7" s="8">
-        <v>68.839285714285708</v>
+        <v>67.592592592592595</v>
       </c>
       <c r="F7" s="8">
-        <v>111.87270501835987</v>
+        <v>97.393364928909961</v>
       </c>
       <c r="G7" s="8">
-        <v>130.24523160762942</v>
+        <v>143.4250764525994</v>
       </c>
       <c r="H7" s="8">
-        <v>97.110754414125196</v>
+        <v>116.50485436893203</v>
       </c>
       <c r="I7" s="8">
-        <v>95.609756097560975</v>
+        <v>100</v>
       </c>
       <c r="J7" s="8">
-        <v>101.25</v>
+        <v>102.33050847457628</v>
       </c>
       <c r="K7" s="8">
-        <v>107.36040609137056</v>
+        <v>102.35294117647058</v>
       </c>
       <c r="L7" s="8">
-        <v>105.94900849858358</v>
+        <v>104.76190476190477</v>
       </c>
       <c r="M7" s="8">
-        <v>110.9375</v>
+        <v>108</v>
       </c>
       <c r="N7" s="8">
-        <v>120.74074074074075</v>
+        <v>109.53846153846155</v>
       </c>
       <c r="O7" s="8">
-        <v>114.81481481481481</v>
+        <v>109.71786833855799</v>
       </c>
       <c r="P7" s="8">
-        <v>117.39130434782609</v>
+        <v>119.9288256227758</v>
       </c>
       <c r="Q7" s="8">
-        <v>97.019867549668874</v>
+        <v>98.226950354609926</v>
       </c>
       <c r="R7" s="8">
-        <v>101.37931034482759</v>
+        <v>97.797356828193841</v>
       </c>
       <c r="S7" s="8">
-        <v>101.12781954887218</v>
+        <v>100.45454545454547</v>
       </c>
       <c r="T7" s="8">
-        <v>98.134328358208961</v>
+        <v>101.03092783505154</v>
       </c>
       <c r="U7" s="8">
-        <v>98.872180451127818</v>
+        <v>97.948717948717942</v>
       </c>
       <c r="V7" s="8">
-        <v>97.5</v>
+        <v>101.88679245283019</v>
       </c>
       <c r="W7" s="8">
-        <v>102.02020202020201</v>
+        <v>98.98989898989899</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
@@ -5980,365 +5963,365 @@
         <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="C8" s="8">
-        <v>85.124956999999995</v>
+        <v>86.703226546906194</v>
       </c>
       <c r="D8" s="8">
-        <v>3.4335260000000001</v>
+        <v>3.339630738522954</v>
       </c>
       <c r="E8" s="8">
-        <v>3.1129009999999999</v>
+        <v>3.3697415169660681</v>
       </c>
       <c r="F8" s="8">
-        <v>2.760529</v>
+        <v>3.0979131736526946</v>
       </c>
       <c r="G8" s="8">
-        <v>2.9914529999999999</v>
+        <v>3.3128253493013973</v>
       </c>
       <c r="H8" s="8">
-        <v>4.4998209999999998</v>
+        <v>4.4911157684630743</v>
       </c>
       <c r="I8" s="8">
-        <v>4.4427089999999998</v>
+        <v>4.9952544910179641</v>
       </c>
       <c r="J8" s="8">
-        <v>5.3014049999999999</v>
+        <v>5.5620439121756489</v>
       </c>
       <c r="K8" s="8">
-        <v>5.7407519999999996</v>
+        <v>5.6074431137724554</v>
       </c>
       <c r="L8" s="8">
-        <v>5.3438040000000004</v>
+        <v>5.4963393213572855</v>
       </c>
       <c r="M8" s="8">
-        <v>5.7348109999999997</v>
+        <v>5.8644351297405191</v>
       </c>
       <c r="N8" s="8">
-        <v>6.2924860000000002</v>
+        <v>5.6470379241516966</v>
       </c>
       <c r="O8" s="8">
-        <v>6.089734</v>
+        <v>5.6964431137724549</v>
       </c>
       <c r="P8" s="8">
-        <v>5.106814</v>
+        <v>5.8456447105788421</v>
       </c>
       <c r="Q8" s="8">
-        <v>4.4891810000000003</v>
+        <v>3.8821177644710581</v>
       </c>
       <c r="R8" s="8">
-        <v>3.8582160000000001</v>
+        <v>3.9730439121756489</v>
       </c>
       <c r="S8" s="8">
-        <v>3.3981569999999999</v>
+        <v>3.2366227544910178</v>
       </c>
       <c r="T8" s="8">
-        <v>3.646439</v>
+        <v>4.0142265469061877</v>
       </c>
       <c r="U8" s="8">
-        <v>2.9765220000000001</v>
+        <v>3.0260648702594812</v>
       </c>
       <c r="V8" s="8">
-        <v>3.2513190000000001</v>
+        <v>3.1581746506986028</v>
       </c>
       <c r="W8" s="8">
-        <v>2.6543779999999999</v>
+        <v>3.0871077844311379</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="C9" s="8">
-        <v>631.5048541665509</v>
+        <v>643.83094228200503</v>
       </c>
       <c r="D9" s="8">
-        <v>28.446854166670004</v>
+        <v>27.173340818351317</v>
       </c>
       <c r="E9" s="8">
-        <v>27.343333333324004</v>
+        <v>28.429807052559884</v>
       </c>
       <c r="F9" s="8">
-        <v>25.958499999969021</v>
+        <v>26.977877578164691</v>
       </c>
       <c r="G9" s="8">
-        <v>26.509166666647001</v>
+        <v>28.429807052545936</v>
       </c>
       <c r="H9" s="8">
-        <v>35.040166666669009</v>
+        <v>33.965984697276461</v>
       </c>
       <c r="I9" s="8">
-        <v>32.299749999987029</v>
+        <v>35.779856952751508</v>
       </c>
       <c r="J9" s="8">
-        <v>33.018249999995</v>
+        <v>31.679890219576826</v>
       </c>
       <c r="K9" s="8">
-        <v>35.559749999995006</v>
+        <v>35.488772455095805</v>
       </c>
       <c r="L9" s="8">
-        <v>33.160166666669994</v>
+        <v>34.328176979363285</v>
       </c>
       <c r="M9" s="8">
-        <v>34.744333333329998</v>
+        <v>35.485861610102802</v>
       </c>
       <c r="N9" s="8">
-        <v>34.32949999999601</v>
+        <v>34.610279441117761</v>
       </c>
       <c r="O9" s="8">
-        <v>34.368916666657007</v>
+        <v>34.618429807045921</v>
       </c>
       <c r="P9" s="8">
-        <v>34.185999999993008</v>
+        <v>35.853043912168673</v>
       </c>
       <c r="Q9" s="8">
-        <v>36.139750000001996</v>
+        <v>33.909431137716574</v>
       </c>
       <c r="R9" s="8">
-        <v>33.614916666673999</v>
+        <v>34.397787757813383</v>
       </c>
       <c r="S9" s="8">
-        <v>33.855166666659009</v>
+        <v>33.799234863601804</v>
       </c>
       <c r="T9" s="8">
-        <v>31.660999999995003</v>
+        <v>35.624750498999006</v>
       </c>
       <c r="U9" s="8">
-        <v>27.220833333327011</v>
+        <v>27.009314703919173</v>
       </c>
       <c r="V9" s="8">
-        <v>28.215999999997006</v>
+        <v>28.159680638718566</v>
       </c>
       <c r="W9" s="8">
-        <v>25.832499999995012</v>
+        <v>28.109614105115785</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="C10" s="8">
-        <v>224.1</v>
+        <v>223.65269461077844</v>
       </c>
       <c r="D10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="E10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="F10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="G10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="H10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="I10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="J10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="K10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="L10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="M10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="N10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="O10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="P10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="Q10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="R10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="S10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="T10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="U10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="V10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
       <c r="W10" s="8">
-        <v>11.205</v>
+        <v>11.182634730538922</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="C11" s="8">
-        <v>12.784260416619999</v>
+        <v>12.758742930776448</v>
       </c>
       <c r="D11" s="8">
-        <v>0.6392604166669994</v>
+        <v>0.63798444776646779</v>
       </c>
       <c r="E11" s="8">
-        <v>0.63874999999400062</v>
+        <v>0.63747504989421155</v>
       </c>
       <c r="F11" s="8">
-        <v>0.64049999997800011</v>
+        <v>0.63922155688722582</v>
       </c>
       <c r="G11" s="8">
-        <v>0.63874999998799986</v>
+        <v>0.63747504989221526</v>
       </c>
       <c r="H11" s="8">
-        <v>0.63875000000400062</v>
+        <v>0.63747504990119797</v>
       </c>
       <c r="I11" s="8">
-        <v>0.63874999999499971</v>
+        <v>0.63747504989620807</v>
       </c>
       <c r="J11" s="8">
-        <v>0.64049999999499962</v>
+        <v>0.63922155688922111</v>
       </c>
       <c r="K11" s="8">
-        <v>0.63875000000099991</v>
+        <v>0.63747504989820414</v>
       </c>
       <c r="L11" s="8">
-        <v>0.63874999999999926</v>
+        <v>0.63747504990119719</v>
       </c>
       <c r="M11" s="8">
-        <v>0.63874999999799986</v>
+        <v>0.63747504990119741</v>
       </c>
       <c r="N11" s="8">
-        <v>0.64050000000100016</v>
+        <v>0.63922155688922166</v>
       </c>
       <c r="O11" s="8">
-        <v>0.63874999999400017</v>
+        <v>0.63747504989520964</v>
       </c>
       <c r="P11" s="8">
-        <v>0.6387499999980002</v>
+        <v>0.63747504990119774</v>
       </c>
       <c r="Q11" s="8">
-        <v>0.63875000000400017</v>
+        <v>0.63747504989620773</v>
       </c>
       <c r="R11" s="8">
-        <v>0.64050000000599971</v>
+        <v>0.63922155688522952</v>
       </c>
       <c r="S11" s="8">
-        <v>0.63874999999899995</v>
+        <v>0.63747504990219561</v>
       </c>
       <c r="T11" s="8">
-        <v>0.638749999997</v>
+        <v>0.63747504989920134</v>
       </c>
       <c r="U11" s="8">
-        <v>0.638749999997</v>
+        <v>0.6374750498992019</v>
       </c>
       <c r="V11" s="8">
-        <v>0.640500000003</v>
+        <v>0.63922155688423143</v>
       </c>
       <c r="W11" s="8">
-        <v>0.63875000000100013</v>
+        <v>0.63747504989720549</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="C12" s="8">
-        <v>12.784260416651</v>
+        <v>12.758742930791419</v>
       </c>
       <c r="D12" s="8">
-        <v>0.63926041667199984</v>
+        <v>0.63798444776546959</v>
       </c>
       <c r="E12" s="8">
-        <v>0.63874999999899984</v>
+        <v>0.63747504990618797</v>
       </c>
       <c r="F12" s="8">
-        <v>0.64049999999400087</v>
+        <v>0.63922155687624793</v>
       </c>
       <c r="G12" s="8">
-        <v>0.63874999999599991</v>
+        <v>0.63747504989720538</v>
       </c>
       <c r="H12" s="8">
-        <v>0.63874999999999982</v>
+        <v>0.63747504990518944</v>
       </c>
       <c r="I12" s="8">
-        <v>0.63874999999500037</v>
+        <v>0.63747504989620773</v>
       </c>
       <c r="J12" s="8">
-        <v>0.64049999999799934</v>
+        <v>0.63922155689720528</v>
       </c>
       <c r="K12" s="8">
-        <v>0.63874999999699988</v>
+        <v>0.63747504991117798</v>
       </c>
       <c r="L12" s="8">
-        <v>0.63875000000699977</v>
+        <v>0.63747504989321324</v>
       </c>
       <c r="M12" s="8">
-        <v>0.63874999999999948</v>
+        <v>0.63747504988922143</v>
       </c>
       <c r="N12" s="8">
-        <v>0.640499999998</v>
+        <v>0.63922155688622773</v>
       </c>
       <c r="O12" s="8">
-        <v>0.63874999999799997</v>
+        <v>0.63747504990019965</v>
       </c>
       <c r="P12" s="8">
-        <v>0.6387499999990004</v>
+        <v>0.63747504989620729</v>
       </c>
       <c r="Q12" s="8">
-        <v>0.63874999999900051</v>
+        <v>0.63747504989820369</v>
       </c>
       <c r="R12" s="8">
-        <v>0.64050000000300011</v>
+        <v>0.63922155688622739</v>
       </c>
       <c r="S12" s="8">
-        <v>0.63874999999799997</v>
+        <v>0.63747504989920167</v>
       </c>
       <c r="T12" s="8">
-        <v>0.63875000000000026</v>
+        <v>0.63747504989920156</v>
       </c>
       <c r="U12" s="8">
-        <v>0.63875000000100024</v>
+        <v>0.63747504989820358</v>
       </c>
       <c r="V12" s="8">
-        <v>0.64049999999699991</v>
+        <v>0.63922155688822369</v>
       </c>
       <c r="W12" s="8">
-        <v>0.63875000000000026</v>
+        <v>0.63747504990219561</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="C13" s="8">
-        <v>3.4580000000000002</v>
+        <v>3.4510978043912175</v>
       </c>
       <c r="D13" s="8">
         <v>0</v>
@@ -6353,43 +6336,43 @@
         <v>0</v>
       </c>
       <c r="H13" s="8">
-        <v>0.26600000000000001</v>
+        <v>0.26546906187624753</v>
       </c>
       <c r="I13" s="8">
-        <v>0.26600000000000001</v>
+        <v>0.26546906187624753</v>
       </c>
       <c r="J13" s="8">
-        <v>0.26600000000000001</v>
+        <v>0.26546906187624753</v>
       </c>
       <c r="K13" s="8">
-        <v>0.26600000000000001</v>
+        <v>0.26546906187624753</v>
       </c>
       <c r="L13" s="8">
-        <v>0.26600000000000001</v>
+        <v>0.26546906187624753</v>
       </c>
       <c r="M13" s="8">
-        <v>0.26600000000000001</v>
+        <v>0.26546906187624753</v>
       </c>
       <c r="N13" s="8">
-        <v>0.26600000000000001</v>
+        <v>0.26546906187624753</v>
       </c>
       <c r="O13" s="8">
-        <v>0.26600000000000001</v>
+        <v>0.26546906187624753</v>
       </c>
       <c r="P13" s="8">
-        <v>0.26600000000000001</v>
+        <v>0.26546906187624753</v>
       </c>
       <c r="Q13" s="8">
-        <v>0.26600000000000001</v>
+        <v>0.26546906187624753</v>
       </c>
       <c r="R13" s="8">
-        <v>0.26600000000000001</v>
+        <v>0.26546906187624753</v>
       </c>
       <c r="S13" s="8">
-        <v>0.26600000000000001</v>
+        <v>0.26546906187624753</v>
       </c>
       <c r="T13" s="8">
-        <v>0.26600000000000001</v>
+        <v>0.26546906187624753</v>
       </c>
       <c r="U13" s="8">
         <v>0</v>
@@ -6403,13 +6386,13 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="C14" s="8">
-        <v>89.375</v>
+        <v>89.876497005988028</v>
       </c>
       <c r="D14" s="8">
         <v>0</v>
@@ -6424,43 +6407,43 @@
         <v>0</v>
       </c>
       <c r="H14" s="8">
-        <v>8.125</v>
+        <v>7.1045409181636723</v>
       </c>
       <c r="I14" s="8">
-        <v>5.0812499999999998</v>
+        <v>7.6783932135728543</v>
       </c>
       <c r="J14" s="8">
-        <v>6.3562500000000002</v>
+        <v>5.0711077844311374</v>
       </c>
       <c r="K14" s="8">
-        <v>8.4812499999999993</v>
+        <v>8.4643213572854297</v>
       </c>
       <c r="L14" s="8">
-        <v>6.5250000000000004</v>
+        <v>6.5119760479041915</v>
       </c>
       <c r="M14" s="8">
-        <v>8.4124999999999996</v>
+        <v>6.8488023952095807</v>
       </c>
       <c r="N14" s="8">
-        <v>8.2624999999999993</v>
+        <v>8.5953093812375254</v>
       </c>
       <c r="O14" s="8">
-        <v>5.0562500000000004</v>
+        <v>5.3642714570858283</v>
       </c>
       <c r="P14" s="8">
-        <v>6.1624999999999996</v>
+        <v>6.5930638722554891</v>
       </c>
       <c r="Q14" s="8">
-        <v>7.3812499999999996</v>
+        <v>5.1210079840319365</v>
       </c>
       <c r="R14" s="8">
-        <v>7.4312500000000004</v>
+        <v>7.4164171656686628</v>
       </c>
       <c r="S14" s="8">
-        <v>6.8</v>
+        <v>6.7864271457085827</v>
       </c>
       <c r="T14" s="8">
-        <v>5.3</v>
+        <v>8.3208582834331342</v>
       </c>
       <c r="U14" s="8">
         <v>0</v>
@@ -6474,84 +6457,84 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="C15" s="8">
-        <v>289.00333333327995</v>
+        <v>301.33316699927946</v>
       </c>
       <c r="D15" s="8">
-        <v>15.963333333331001</v>
+        <v>14.714737192280438</v>
       </c>
       <c r="E15" s="8">
-        <v>14.860833333331001</v>
+        <v>15.972222222220561</v>
       </c>
       <c r="F15" s="8">
-        <v>13.472499999996998</v>
+        <v>14.516799733862273</v>
       </c>
       <c r="G15" s="8">
-        <v>14.026666666662999</v>
+        <v>15.972222222217566</v>
       </c>
       <c r="H15" s="8">
-        <v>14.166666666665005</v>
+        <v>14.138389886891222</v>
       </c>
       <c r="I15" s="8">
-        <v>14.469999999997</v>
+        <v>15.378409846971056</v>
       </c>
       <c r="J15" s="8">
-        <v>13.910000000002002</v>
+        <v>13.882235528944115</v>
       </c>
       <c r="K15" s="8">
-        <v>14.329999999997002</v>
+        <v>14.301397205585829</v>
       </c>
       <c r="L15" s="8">
-        <v>13.886666666662999</v>
+        <v>15.093147039249502</v>
       </c>
       <c r="M15" s="8">
-        <v>13.583333333332</v>
+        <v>15.914005322687624</v>
       </c>
       <c r="N15" s="8">
-        <v>13.314999999996997</v>
+        <v>13.288423153689617</v>
       </c>
       <c r="O15" s="8">
-        <v>16.564166666665006</v>
+        <v>16.531104457749507</v>
       </c>
       <c r="P15" s="8">
-        <v>15.274999999995995</v>
+        <v>16.536926147700594</v>
       </c>
       <c r="Q15" s="8">
-        <v>16.009999999999003</v>
+        <v>16.065369261475052</v>
       </c>
       <c r="R15" s="8">
-        <v>13.431666666664999</v>
+        <v>14.254823685958085</v>
       </c>
       <c r="S15" s="8">
-        <v>14.306666666662</v>
+        <v>14.289753825676648</v>
       </c>
       <c r="T15" s="8">
-        <v>13.612499999997999</v>
+        <v>14.580838323352292</v>
       </c>
       <c r="U15" s="8">
-        <v>14.738333333329003</v>
+        <v>14.55172987358284</v>
       </c>
       <c r="V15" s="8">
-        <v>15.729999999996997</v>
+        <v>15.698602794407185</v>
       </c>
       <c r="W15" s="8">
-        <v>13.349999999993999</v>
+        <v>15.652029274777444</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B16" t="s">
         <v>96</v>
       </c>
       <c r="C16" s="8">
-        <v>0.42987641053197206</v>
+        <v>0.16120365394948952</v>
       </c>
       <c r="D16" s="8">
         <v>0</v>
@@ -6572,7 +6555,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="8">
-        <v>0</v>
+        <v>3.225806451612903</v>
       </c>
       <c r="K16" s="8">
         <v>0</v>
@@ -6584,13 +6567,13 @@
         <v>0</v>
       </c>
       <c r="N16" s="8">
-        <v>4.3010752688172049</v>
+        <v>0</v>
       </c>
       <c r="O16" s="8">
         <v>0</v>
       </c>
       <c r="P16" s="8">
-        <v>4.3010752688172049</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="8">
         <v>0</v>
@@ -6616,13 +6599,13 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B17" t="s">
         <v>96</v>
       </c>
       <c r="C17" s="8">
-        <v>6.6529774127310066</v>
+        <v>3.9425051334702261</v>
       </c>
       <c r="D17" s="8">
         <v>0</v>
@@ -6643,7 +6626,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="8">
-        <v>0</v>
+        <v>78.688524590163937</v>
       </c>
       <c r="K17" s="8">
         <v>0</v>
@@ -6655,13 +6638,13 @@
         <v>0</v>
       </c>
       <c r="N17" s="8">
-        <v>75.136612021857914</v>
+        <v>0</v>
       </c>
       <c r="O17" s="8">
         <v>0</v>
       </c>
       <c r="P17" s="8">
-        <v>57.80821917808219</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="8">
         <v>0</v>
@@ -6687,13 +6670,13 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B18" t="s">
         <v>96</v>
       </c>
       <c r="C18" s="8">
-        <v>6.5845311430527032</v>
+        <v>3.9425051334702261</v>
       </c>
       <c r="D18" s="8">
         <v>0</v>
@@ -6714,7 +6697,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="8">
-        <v>0</v>
+        <v>78.688524590163937</v>
       </c>
       <c r="K18" s="8">
         <v>0</v>
@@ -6726,13 +6709,13 @@
         <v>0</v>
       </c>
       <c r="N18" s="8">
-        <v>75.136612021857914</v>
+        <v>0</v>
       </c>
       <c r="O18" s="8">
         <v>0</v>
       </c>
       <c r="P18" s="8">
-        <v>56.438356164383563</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="8">
         <v>0</v>
@@ -6758,7 +6741,7 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B19" t="s">
         <v>96</v>
@@ -6829,13 +6812,13 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B20" t="s">
         <v>96</v>
       </c>
       <c r="C20" s="8">
-        <v>7.4600355239786849</v>
+        <v>2.2847100175746924</v>
       </c>
       <c r="D20" s="8">
         <v>0</v>
@@ -6856,7 +6839,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="8">
-        <v>0</v>
+        <v>41.935483870967744</v>
       </c>
       <c r="K20" s="8">
         <v>0</v>
@@ -6868,13 +6851,13 @@
         <v>0</v>
       </c>
       <c r="N20" s="8">
-        <v>46.153846153846153</v>
+        <v>0</v>
       </c>
       <c r="O20" s="8">
         <v>0</v>
       </c>
       <c r="P20" s="8">
-        <v>46.153846153846153</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="8">
         <v>0</v>
@@ -6900,13 +6883,13 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B21" t="s">
         <v>96</v>
       </c>
       <c r="C21" s="8">
-        <v>9.0196078431372548</v>
+        <v>4.1725269573370838</v>
       </c>
       <c r="D21" s="8">
         <v>0</v>
@@ -6927,7 +6910,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="8">
-        <v>0</v>
+        <v>90.816326530612244</v>
       </c>
       <c r="K21" s="8">
         <v>0</v>
@@ -6939,13 +6922,13 @@
         <v>0</v>
       </c>
       <c r="N21" s="8">
-        <v>94.680851063829792</v>
+        <v>0</v>
       </c>
       <c r="O21" s="8">
         <v>0</v>
       </c>
       <c r="P21" s="8">
-        <v>87.962962962962962</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="8">
         <v>0</v>

</xml_diff>